<commit_message>
Run each observation through appropriate species model
i.e if an observation is for 'Mouse' it will run the observation via the 'mouse' model
</commit_message>
<xml_diff>
--- a/sample_output.xlsx
+++ b/sample_output.xlsx
@@ -1,15 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellechandrasaputra/Documents/Monash/2019/FIT3162-Team21/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D83FFCA-E3E4-EA49-9C92-922BB41A7197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -118,8 +132,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +170,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -202,7 +224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,9 +256,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,6 +308,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,14 +501,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,22 +590,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>11028</v>
+        <v>60555</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C2" t="e">
         <f>#NUM!</f>
         <v>#NUM!</v>
       </c>
       <c r="D2">
-        <v>-38.35692</v>
+        <v>-38.356920000000002</v>
       </c>
       <c r="E2">
-        <v>144.97151</v>
+        <v>144.97150999999999</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -563,28 +623,28 @@
         <v>2229.56396484375</v>
       </c>
       <c r="K2">
-        <v>74.74870300292969</v>
+        <v>74.748703002929688</v>
       </c>
       <c r="L2">
-        <v>89.66790008544922</v>
+        <v>89.667900085449219</v>
       </c>
       <c r="M2">
-        <v>74.74870300292969</v>
+        <v>74.748703002929688</v>
       </c>
       <c r="N2">
-        <v>251.6891021728516</v>
+        <v>251.68910217285159</v>
       </c>
       <c r="O2">
-        <v>7.762680530548096</v>
+        <v>7.7626805305480957</v>
       </c>
       <c r="P2">
-        <v>0.3700941205024719</v>
+        <v>0.37009412050247192</v>
       </c>
       <c r="Q2">
-        <v>0.06840000301599503</v>
+        <v>6.8400003015995026E-2</v>
       </c>
       <c r="R2">
-        <v>2.337699890136719</v>
+        <v>2.3376998901367192</v>
       </c>
       <c r="S2">
         <v>6</v>
@@ -602,16 +662,16 @@
         <v>146</v>
       </c>
       <c r="X2">
-        <v>-0.3797000050544739</v>
+        <v>-0.37970000505447388</v>
       </c>
       <c r="Y2">
-        <v>216.1999969482422</v>
+        <v>216.19999694824219</v>
       </c>
       <c r="Z2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11028</v>
       </c>
@@ -623,10 +683,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D3">
-        <v>-38.35598</v>
+        <v>-38.355980000000002</v>
       </c>
       <c r="E3">
-        <v>144.96925</v>
+        <v>144.96924999999999</v>
       </c>
       <c r="F3" t="s">
         <v>27</v>
@@ -644,28 +704,28 @@
         <v>2270.537353515625</v>
       </c>
       <c r="K3">
-        <v>78.06990051269531</v>
+        <v>78.069900512695312</v>
       </c>
       <c r="L3">
-        <v>86.32180023193359</v>
+        <v>86.321800231933594</v>
       </c>
       <c r="M3">
-        <v>78.06990051269531</v>
+        <v>78.069900512695312</v>
       </c>
       <c r="N3">
         <v>247.9299011230469</v>
       </c>
       <c r="O3">
-        <v>9.545023918151855</v>
+        <v>9.5450239181518555</v>
       </c>
       <c r="P3">
-        <v>0.5925191044807434</v>
+        <v>0.59251910448074341</v>
       </c>
       <c r="Q3">
-        <v>0.03030000068247318</v>
+        <v>3.0300000682473179E-2</v>
       </c>
       <c r="R3">
-        <v>2.384200096130371</v>
+        <v>2.3842000961303711</v>
       </c>
       <c r="S3">
         <v>106</v>
@@ -674,7 +734,7 @@
         <v>118</v>
       </c>
       <c r="U3">
-        <v>0.03198285028338432</v>
+        <v>3.1982850283384323E-2</v>
       </c>
       <c r="V3">
         <v>45</v>
@@ -683,16 +743,16 @@
         <v>136</v>
       </c>
       <c r="X3">
-        <v>0.009800000116229057</v>
+        <v>9.8000001162290573E-3</v>
       </c>
       <c r="Y3">
-        <v>240.8000030517578</v>
+        <v>240.80000305175781</v>
       </c>
       <c r="Z3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>11028</v>
       </c>
@@ -704,10 +764,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D4">
-        <v>-38.35598</v>
+        <v>-38.355980000000002</v>
       </c>
       <c r="E4">
-        <v>144.96925</v>
+        <v>144.96924999999999</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -725,28 +785,28 @@
         <v>2270.537353515625</v>
       </c>
       <c r="K4">
-        <v>78.06990051269531</v>
+        <v>78.069900512695312</v>
       </c>
       <c r="L4">
-        <v>86.32180023193359</v>
+        <v>86.321800231933594</v>
       </c>
       <c r="M4">
-        <v>78.06990051269531</v>
+        <v>78.069900512695312</v>
       </c>
       <c r="N4">
         <v>247.9299011230469</v>
       </c>
       <c r="O4">
-        <v>9.545023918151855</v>
+        <v>9.5450239181518555</v>
       </c>
       <c r="P4">
-        <v>0.5925191044807434</v>
+        <v>0.59251910448074341</v>
       </c>
       <c r="Q4">
-        <v>0.03030000068247318</v>
+        <v>3.0300000682473179E-2</v>
       </c>
       <c r="R4">
-        <v>2.384200096130371</v>
+        <v>2.3842000961303711</v>
       </c>
       <c r="S4">
         <v>106</v>
@@ -755,7 +815,7 @@
         <v>118</v>
       </c>
       <c r="U4">
-        <v>0.03198285028338432</v>
+        <v>3.1982850283384323E-2</v>
       </c>
       <c r="V4">
         <v>45</v>
@@ -764,16 +824,16 @@
         <v>136</v>
       </c>
       <c r="X4">
-        <v>0.009800000116229057</v>
+        <v>9.8000001162290573E-3</v>
       </c>
       <c r="Y4">
-        <v>240.8000030517578</v>
+        <v>240.80000305175781</v>
       </c>
       <c r="Z4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11028</v>
       </c>
@@ -785,10 +845,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D5">
-        <v>-37.28102</v>
+        <v>-37.281019999999998</v>
       </c>
       <c r="E5">
-        <v>143.07973</v>
+        <v>143.07973000000001</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
@@ -806,28 +866,28 @@
         <v>1878.319580078125</v>
       </c>
       <c r="K5">
-        <v>35.53960037231445</v>
+        <v>35.539600372314453</v>
       </c>
       <c r="L5">
-        <v>64.69170379638672</v>
+        <v>64.691703796386719</v>
       </c>
       <c r="M5">
-        <v>35.53960037231445</v>
+        <v>35.539600372314453</v>
       </c>
       <c r="N5">
-        <v>296.5842895507812</v>
+        <v>296.58428955078119</v>
       </c>
       <c r="O5">
-        <v>9.601596832275391</v>
+        <v>9.6015968322753906</v>
       </c>
       <c r="P5">
-        <v>3.710224390029907</v>
+        <v>3.7102243900299068</v>
       </c>
       <c r="Q5">
-        <v>0.05180000141263008</v>
+        <v>5.1800001412630081E-2</v>
       </c>
       <c r="R5">
-        <v>2.336199998855591</v>
+        <v>2.3361999988555908</v>
       </c>
       <c r="S5">
         <v>3</v>
@@ -836,7 +896,7 @@
         <v>100</v>
       </c>
       <c r="U5">
-        <v>0.02477074041962624</v>
+        <v>2.4770740419626239E-2</v>
       </c>
       <c r="V5">
         <v>38</v>
@@ -845,7 +905,7 @@
         <v>91</v>
       </c>
       <c r="X5">
-        <v>0.859000027179718</v>
+        <v>0.85900002717971802</v>
       </c>
       <c r="Y5">
         <v>423</v>
@@ -854,7 +914,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>11028</v>
       </c>
@@ -866,7 +926,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D6">
-        <v>-37.68834</v>
+        <v>-37.688339999999997</v>
       </c>
       <c r="E6">
         <v>145.52175</v>
@@ -887,25 +947,25 @@
         <v>2262.26904296875</v>
       </c>
       <c r="K6">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="L6">
-        <v>81.63500213623047</v>
+        <v>81.635002136230469</v>
       </c>
       <c r="M6">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="N6">
-        <v>298.2625122070312</v>
+        <v>298.26251220703119</v>
       </c>
       <c r="O6">
-        <v>10.10383701324463</v>
+        <v>10.103837013244631</v>
       </c>
       <c r="P6">
-        <v>0.9190149307250977</v>
+        <v>0.91901493072509766</v>
       </c>
       <c r="Q6">
-        <v>0.06629999727010727</v>
+        <v>6.6299997270107269E-2</v>
       </c>
       <c r="R6">
         <v>1.883900046348572</v>
@@ -917,7 +977,7 @@
         <v>106</v>
       </c>
       <c r="U6">
-        <v>0.5543010830879211</v>
+        <v>0.55430108308792114</v>
       </c>
       <c r="V6">
         <v>40</v>
@@ -926,16 +986,16 @@
         <v>30</v>
       </c>
       <c r="X6">
-        <v>-0.2379000037908554</v>
+        <v>-0.23790000379085541</v>
       </c>
       <c r="Y6">
-        <v>95.19999694824219</v>
+        <v>95.199996948242188</v>
       </c>
       <c r="Z6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11028</v>
       </c>
@@ -947,7 +1007,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D7">
-        <v>-37.68834</v>
+        <v>-37.688339999999997</v>
       </c>
       <c r="E7">
         <v>145.52175</v>
@@ -968,25 +1028,25 @@
         <v>2262.26904296875</v>
       </c>
       <c r="K7">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="L7">
-        <v>81.63500213623047</v>
+        <v>81.635002136230469</v>
       </c>
       <c r="M7">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="N7">
-        <v>298.2625122070312</v>
+        <v>298.26251220703119</v>
       </c>
       <c r="O7">
-        <v>10.10383701324463</v>
+        <v>10.103837013244631</v>
       </c>
       <c r="P7">
-        <v>0.9190149307250977</v>
+        <v>0.91901493072509766</v>
       </c>
       <c r="Q7">
-        <v>0.06629999727010727</v>
+        <v>6.6299997270107269E-2</v>
       </c>
       <c r="R7">
         <v>1.883900046348572</v>
@@ -998,7 +1058,7 @@
         <v>106</v>
       </c>
       <c r="U7">
-        <v>0.5543010830879211</v>
+        <v>0.55430108308792114</v>
       </c>
       <c r="V7">
         <v>40</v>
@@ -1007,16 +1067,16 @@
         <v>30</v>
       </c>
       <c r="X7">
-        <v>-0.2379000037908554</v>
+        <v>-0.23790000379085541</v>
       </c>
       <c r="Y7">
-        <v>95.19999694824219</v>
+        <v>95.199996948242188</v>
       </c>
       <c r="Z7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>11028</v>
       </c>
@@ -1028,7 +1088,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D8">
-        <v>-37.68834</v>
+        <v>-37.688339999999997</v>
       </c>
       <c r="E8">
         <v>145.52175</v>
@@ -1049,25 +1109,25 @@
         <v>2262.26904296875</v>
       </c>
       <c r="K8">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="L8">
-        <v>81.63500213623047</v>
+        <v>81.635002136230469</v>
       </c>
       <c r="M8">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="N8">
-        <v>298.2625122070312</v>
+        <v>298.26251220703119</v>
       </c>
       <c r="O8">
-        <v>10.10383701324463</v>
+        <v>10.103837013244631</v>
       </c>
       <c r="P8">
-        <v>0.9190149307250977</v>
+        <v>0.91901493072509766</v>
       </c>
       <c r="Q8">
-        <v>0.06629999727010727</v>
+        <v>6.6299997270107269E-2</v>
       </c>
       <c r="R8">
         <v>1.883900046348572</v>
@@ -1079,7 +1139,7 @@
         <v>106</v>
       </c>
       <c r="U8">
-        <v>0.5543010830879211</v>
+        <v>0.55430108308792114</v>
       </c>
       <c r="V8">
         <v>40</v>
@@ -1088,16 +1148,16 @@
         <v>30</v>
       </c>
       <c r="X8">
-        <v>-0.2379000037908554</v>
+        <v>-0.23790000379085541</v>
       </c>
       <c r="Y8">
-        <v>95.19999694824219</v>
+        <v>95.199996948242188</v>
       </c>
       <c r="Z8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>11028</v>
       </c>
@@ -1109,7 +1169,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D9">
-        <v>-37.68834</v>
+        <v>-37.688339999999997</v>
       </c>
       <c r="E9">
         <v>145.52175</v>
@@ -1130,25 +1190,25 @@
         <v>2262.26904296875</v>
       </c>
       <c r="K9">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="L9">
-        <v>81.63500213623047</v>
+        <v>81.635002136230469</v>
       </c>
       <c r="M9">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="N9">
-        <v>298.2625122070312</v>
+        <v>298.26251220703119</v>
       </c>
       <c r="O9">
-        <v>10.10383701324463</v>
+        <v>10.103837013244631</v>
       </c>
       <c r="P9">
-        <v>0.9190149307250977</v>
+        <v>0.91901493072509766</v>
       </c>
       <c r="Q9">
-        <v>0.06629999727010727</v>
+        <v>6.6299997270107269E-2</v>
       </c>
       <c r="R9">
         <v>1.883900046348572</v>
@@ -1160,7 +1220,7 @@
         <v>106</v>
       </c>
       <c r="U9">
-        <v>0.5543010830879211</v>
+        <v>0.55430108308792114</v>
       </c>
       <c r="V9">
         <v>40</v>
@@ -1169,16 +1229,16 @@
         <v>30</v>
       </c>
       <c r="X9">
-        <v>-0.2379000037908554</v>
+        <v>-0.23790000379085541</v>
       </c>
       <c r="Y9">
-        <v>95.19999694824219</v>
+        <v>95.199996948242188</v>
       </c>
       <c r="Z9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>11028</v>
       </c>
@@ -1190,7 +1250,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D10">
-        <v>-37.68834</v>
+        <v>-37.688339999999997</v>
       </c>
       <c r="E10">
         <v>145.52175</v>
@@ -1211,25 +1271,25 @@
         <v>2262.26904296875</v>
       </c>
       <c r="K10">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="L10">
-        <v>81.63500213623047</v>
+        <v>81.635002136230469</v>
       </c>
       <c r="M10">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="N10">
-        <v>298.2625122070312</v>
+        <v>298.26251220703119</v>
       </c>
       <c r="O10">
-        <v>10.10383701324463</v>
+        <v>10.103837013244631</v>
       </c>
       <c r="P10">
-        <v>0.9190149307250977</v>
+        <v>0.91901493072509766</v>
       </c>
       <c r="Q10">
-        <v>0.06629999727010727</v>
+        <v>6.6299997270107269E-2</v>
       </c>
       <c r="R10">
         <v>1.883900046348572</v>
@@ -1241,7 +1301,7 @@
         <v>106</v>
       </c>
       <c r="U10">
-        <v>0.5543010830879211</v>
+        <v>0.55430108308792114</v>
       </c>
       <c r="V10">
         <v>40</v>
@@ -1250,16 +1310,16 @@
         <v>30</v>
       </c>
       <c r="X10">
-        <v>-0.2379000037908554</v>
+        <v>-0.23790000379085541</v>
       </c>
       <c r="Y10">
-        <v>95.19999694824219</v>
+        <v>95.199996948242188</v>
       </c>
       <c r="Z10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11028</v>
       </c>
@@ -1271,7 +1331,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D11">
-        <v>-37.68834</v>
+        <v>-37.688339999999997</v>
       </c>
       <c r="E11">
         <v>145.52175</v>
@@ -1292,25 +1352,25 @@
         <v>2262.26904296875</v>
       </c>
       <c r="K11">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="L11">
-        <v>81.63500213623047</v>
+        <v>81.635002136230469</v>
       </c>
       <c r="M11">
-        <v>51.60449981689453</v>
+        <v>51.604499816894531</v>
       </c>
       <c r="N11">
-        <v>298.2625122070312</v>
+        <v>298.26251220703119</v>
       </c>
       <c r="O11">
-        <v>10.10383701324463</v>
+        <v>10.103837013244631</v>
       </c>
       <c r="P11">
-        <v>0.9190149307250977</v>
+        <v>0.91901493072509766</v>
       </c>
       <c r="Q11">
-        <v>0.06629999727010727</v>
+        <v>6.6299997270107269E-2</v>
       </c>
       <c r="R11">
         <v>1.883900046348572</v>
@@ -1322,7 +1382,7 @@
         <v>106</v>
       </c>
       <c r="U11">
-        <v>0.5543010830879211</v>
+        <v>0.55430108308792114</v>
       </c>
       <c r="V11">
         <v>40</v>
@@ -1331,16 +1391,16 @@
         <v>30</v>
       </c>
       <c r="X11">
-        <v>-0.2379000037908554</v>
+        <v>-0.23790000379085541</v>
       </c>
       <c r="Y11">
-        <v>95.19999694824219</v>
+        <v>95.199996948242188</v>
       </c>
       <c r="Z11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11028</v>
       </c>
@@ -1352,7 +1412,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D12">
-        <v>-37.95565</v>
+        <v>-37.955649999999999</v>
       </c>
       <c r="E12">
         <v>145.49364</v>
@@ -1373,28 +1433,28 @@
         <v>2673.4814453125</v>
       </c>
       <c r="K12">
-        <v>71.55020141601562</v>
+        <v>71.550201416015625</v>
       </c>
       <c r="L12">
-        <v>72.70400238037109</v>
+        <v>72.704002380371094</v>
       </c>
       <c r="M12">
-        <v>71.55020141601562</v>
+        <v>71.550201416015625</v>
       </c>
       <c r="N12">
-        <v>271.3330993652344</v>
+        <v>271.33309936523438</v>
       </c>
       <c r="O12">
-        <v>11.7710485458374</v>
+        <v>11.771048545837401</v>
       </c>
       <c r="P12">
-        <v>0.753390908241272</v>
+        <v>0.75339090824127197</v>
       </c>
       <c r="Q12">
-        <v>0.03280000016093254</v>
+        <v>3.2800000160932541E-2</v>
       </c>
       <c r="R12">
-        <v>2.476599931716919</v>
+        <v>2.4765999317169189</v>
       </c>
       <c r="S12">
         <v>16</v>
@@ -1403,7 +1463,7 @@
         <v>124</v>
       </c>
       <c r="U12">
-        <v>0.03266274183988571</v>
+        <v>3.2662741839885712E-2</v>
       </c>
       <c r="V12">
         <v>62</v>
@@ -1412,7 +1472,7 @@
         <v>98</v>
       </c>
       <c r="X12">
-        <v>-0.3851999938488007</v>
+        <v>-0.38519999384880071</v>
       </c>
       <c r="Y12">
         <v>308</v>
@@ -1421,7 +1481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11028</v>
       </c>
@@ -1433,7 +1493,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D13">
-        <v>-37.95565</v>
+        <v>-37.955649999999999</v>
       </c>
       <c r="E13">
         <v>145.49364</v>
@@ -1454,28 +1514,28 @@
         <v>2673.4814453125</v>
       </c>
       <c r="K13">
-        <v>71.55020141601562</v>
+        <v>71.550201416015625</v>
       </c>
       <c r="L13">
-        <v>72.70400238037109</v>
+        <v>72.704002380371094</v>
       </c>
       <c r="M13">
-        <v>71.55020141601562</v>
+        <v>71.550201416015625</v>
       </c>
       <c r="N13">
-        <v>271.3330993652344</v>
+        <v>271.33309936523438</v>
       </c>
       <c r="O13">
-        <v>11.7710485458374</v>
+        <v>11.771048545837401</v>
       </c>
       <c r="P13">
-        <v>0.753390908241272</v>
+        <v>0.75339090824127197</v>
       </c>
       <c r="Q13">
-        <v>0.03280000016093254</v>
+        <v>3.2800000160932541E-2</v>
       </c>
       <c r="R13">
-        <v>2.476599931716919</v>
+        <v>2.4765999317169189</v>
       </c>
       <c r="S13">
         <v>16</v>
@@ -1484,7 +1544,7 @@
         <v>124</v>
       </c>
       <c r="U13">
-        <v>0.03266274183988571</v>
+        <v>3.2662741839885712E-2</v>
       </c>
       <c r="V13">
         <v>62</v>
@@ -1493,7 +1553,7 @@
         <v>98</v>
       </c>
       <c r="X13">
-        <v>-0.3851999938488007</v>
+        <v>-0.38519999384880071</v>
       </c>
       <c r="Y13">
         <v>308</v>
@@ -1502,7 +1562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11028</v>
       </c>
@@ -1514,10 +1574,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D14">
-        <v>-37.36868</v>
+        <v>-37.368679999999998</v>
       </c>
       <c r="E14">
-        <v>145.27735</v>
+        <v>145.27735000000001</v>
       </c>
       <c r="F14" t="s">
         <v>29</v>
@@ -1526,7 +1586,7 @@
         <v>12</v>
       </c>
       <c r="H14">
-        <v>14.91030025482178</v>
+        <v>14.910300254821779</v>
       </c>
       <c r="I14">
         <v>1839.2548828125</v>
@@ -1535,28 +1595,28 @@
         <v>1794.35498046875</v>
       </c>
       <c r="K14">
-        <v>49.02890014648438</v>
+        <v>49.028900146484382</v>
       </c>
       <c r="L14">
-        <v>68.41049957275391</v>
+        <v>68.410499572753906</v>
       </c>
       <c r="M14">
-        <v>49.02890014648438</v>
+        <v>49.028900146484382</v>
       </c>
       <c r="N14">
         <v>293.360595703125</v>
       </c>
       <c r="O14">
-        <v>10.90413093566895</v>
+        <v>10.904130935668951</v>
       </c>
       <c r="P14">
-        <v>1.142726540565491</v>
+        <v>1.1427265405654909</v>
       </c>
       <c r="Q14">
-        <v>0.1187999993562698</v>
+        <v>0.11879999935626979</v>
       </c>
       <c r="R14">
-        <v>2.474499940872192</v>
+        <v>2.4744999408721919</v>
       </c>
       <c r="S14">
         <v>12</v>
@@ -1565,7 +1625,7 @@
         <v>102</v>
       </c>
       <c r="U14">
-        <v>0.04459736123681068</v>
+        <v>4.4597361236810677E-2</v>
       </c>
       <c r="V14">
         <v>53</v>
@@ -1574,16 +1634,16 @@
         <v>6</v>
       </c>
       <c r="X14">
-        <v>-0.3061999976634979</v>
+        <v>-0.30619999766349792</v>
       </c>
       <c r="Y14">
-        <v>334.3999938964844</v>
+        <v>334.39999389648438</v>
       </c>
       <c r="Z14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11028</v>
       </c>
@@ -1595,10 +1655,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D15">
-        <v>-37.06096</v>
+        <v>-37.060960000000001</v>
       </c>
       <c r="E15">
-        <v>146.74537</v>
+        <v>146.74537000000001</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
@@ -1616,25 +1676,25 @@
         <v>1957.339477539062</v>
       </c>
       <c r="K15">
-        <v>142.6916046142578</v>
+        <v>142.69160461425781</v>
       </c>
       <c r="L15">
-        <v>35.22639846801758</v>
+        <v>35.226398468017578</v>
       </c>
       <c r="M15">
-        <v>142.6916046142578</v>
+        <v>142.69160461425781</v>
       </c>
       <c r="N15">
-        <v>267.1351928710938</v>
+        <v>267.13519287109381</v>
       </c>
       <c r="O15">
-        <v>10.92054843902588</v>
+        <v>10.920548439025881</v>
       </c>
       <c r="P15">
-        <v>0.8346856236457825</v>
+        <v>0.83468562364578247</v>
       </c>
       <c r="Q15">
-        <v>0.03620000183582306</v>
+        <v>3.6200001835823059E-2</v>
       </c>
       <c r="R15">
         <v>2.961999893188477</v>
@@ -1646,7 +1706,7 @@
         <v>88</v>
       </c>
       <c r="U15">
-        <v>0.004344508051872253</v>
+        <v>4.3445080518722534E-3</v>
       </c>
       <c r="V15">
         <v>4</v>
@@ -1655,16 +1715,16 @@
         <v>101</v>
       </c>
       <c r="X15">
-        <v>-1.197000026702881</v>
+        <v>-1.1970000267028811</v>
       </c>
       <c r="Y15">
-        <v>937.2000122070312</v>
+        <v>937.20001220703125</v>
       </c>
       <c r="Z15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>503998</v>
       </c>
@@ -1676,10 +1736,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D16">
-        <v>-37.00972</v>
+        <v>-37.009720000000002</v>
       </c>
       <c r="E16">
-        <v>142.72417</v>
+        <v>142.72416999999999</v>
       </c>
       <c r="F16" t="e">
         <f>#NUM!</f>
@@ -1689,7 +1749,7 @@
         <v>6</v>
       </c>
       <c r="H16">
-        <v>16.25909996032715</v>
+        <v>16.259099960327148</v>
       </c>
       <c r="I16">
         <v>2000.8466796875</v>
@@ -1698,16 +1758,16 @@
         <v>1933.119750976562</v>
       </c>
       <c r="K16">
-        <v>28.68449974060059</v>
+        <v>28.684499740600589</v>
       </c>
       <c r="L16">
-        <v>73.31549835205078</v>
+        <v>73.315498352050781</v>
       </c>
       <c r="M16">
-        <v>28.68449974060059</v>
+        <v>28.684499740600589</v>
       </c>
       <c r="N16">
-        <v>317.3330993652344</v>
+        <v>317.33309936523438</v>
       </c>
       <c r="O16">
         <v>13.97187423706055</v>
@@ -1716,10 +1776,10 @@
         <v>0.1023558080196381</v>
       </c>
       <c r="Q16">
-        <v>0.001000000047497451</v>
+        <v>1.0000000474974511E-3</v>
       </c>
       <c r="R16">
-        <v>1.881999969482422</v>
+        <v>1.8819999694824221</v>
       </c>
       <c r="S16">
         <v>6</v>
@@ -1728,7 +1788,7 @@
         <v>96</v>
       </c>
       <c r="U16">
-        <v>0.07739999890327454</v>
+        <v>7.7399998903274536E-2</v>
       </c>
       <c r="V16">
         <v>35</v>
@@ -1737,16 +1797,16 @@
         <v>121</v>
       </c>
       <c r="X16">
-        <v>0.0003000000142492354</v>
+        <v>3.0000001424923539E-4</v>
       </c>
       <c r="Y16">
-        <v>231.8000030517578</v>
+        <v>231.80000305175781</v>
       </c>
       <c r="Z16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>60555</v>
       </c>
@@ -1770,7 +1830,7 @@
         <v>4</v>
       </c>
       <c r="H17">
-        <v>16.08259963989258</v>
+        <v>16.082599639892582</v>
       </c>
       <c r="I17">
         <v>2207.20458984375</v>
@@ -1782,25 +1842,25 @@
         <v>-1.658499956130981</v>
       </c>
       <c r="L17">
-        <v>70.65850067138672</v>
+        <v>70.658500671386719</v>
       </c>
       <c r="M17">
         <v>-1.658499956130981</v>
       </c>
       <c r="N17">
-        <v>340.5935974121094</v>
+        <v>340.59359741210938</v>
       </c>
       <c r="O17">
-        <v>5.18536901473999</v>
+        <v>5.1853690147399902</v>
       </c>
       <c r="P17">
-        <v>0.6785849332809448</v>
+        <v>0.67858493328094482</v>
       </c>
       <c r="Q17">
-        <v>0.003700000001117587</v>
+        <v>3.7000000011175871E-3</v>
       </c>
       <c r="R17">
-        <v>1.042500019073486</v>
+        <v>1.0425000190734861</v>
       </c>
       <c r="S17">
         <v>18</v>
@@ -1809,7 +1869,7 @@
         <v>37</v>
       </c>
       <c r="U17">
-        <v>0.02453536912798882</v>
+        <v>2.4535369127988819E-2</v>
       </c>
       <c r="V17">
         <v>29</v>
@@ -1818,16 +1878,16 @@
         <v>11</v>
       </c>
       <c r="X17">
-        <v>-0.0003999999898951501</v>
+        <v>-3.9999998989515012E-4</v>
       </c>
       <c r="Y17">
-        <v>65.51249694824219</v>
+        <v>65.512496948242188</v>
       </c>
       <c r="Z17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>60555</v>
       </c>
@@ -1839,10 +1899,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D18">
-        <v>-34.7162</v>
+        <v>-34.716200000000001</v>
       </c>
       <c r="E18">
-        <v>141.6648</v>
+        <v>141.66480000000001</v>
       </c>
       <c r="F18" t="s">
         <v>29</v>
@@ -1860,28 +1920,28 @@
         <v>2081.8896484375</v>
       </c>
       <c r="K18">
-        <v>-0.6797000169754028</v>
+        <v>-0.67970001697540283</v>
       </c>
       <c r="L18">
         <v>67.13800048828125</v>
       </c>
       <c r="M18">
-        <v>-0.6797000169754028</v>
+        <v>-0.67970001697540283</v>
       </c>
       <c r="N18">
-        <v>342.1380004882812</v>
+        <v>342.13800048828119</v>
       </c>
       <c r="O18">
         <v>3.420849084854126</v>
       </c>
       <c r="P18">
-        <v>0.2342628985643387</v>
+        <v>0.23426289856433871</v>
       </c>
       <c r="Q18">
-        <v>0.005299999844282866</v>
+        <v>5.2999998442828664E-3</v>
       </c>
       <c r="R18">
-        <v>1.536800026893616</v>
+        <v>1.5368000268936159</v>
       </c>
       <c r="S18">
         <v>5</v>
@@ -1890,7 +1950,7 @@
         <v>42</v>
       </c>
       <c r="U18">
-        <v>0.01290467008948326</v>
+        <v>1.2904670089483259E-2</v>
       </c>
       <c r="V18">
         <v>72</v>
@@ -1899,16 +1959,16 @@
         <v>88</v>
       </c>
       <c r="X18">
-        <v>-0.003700000001117587</v>
+        <v>-3.7000000011175871E-3</v>
       </c>
       <c r="Y18">
-        <v>69.40000152587891</v>
+        <v>69.400001525878906</v>
       </c>
       <c r="Z18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>60555</v>
       </c>
@@ -1920,10 +1980,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D19">
-        <v>-36.6977</v>
+        <v>-36.697699999999998</v>
       </c>
       <c r="E19">
-        <v>142.633</v>
+        <v>142.63300000000001</v>
       </c>
       <c r="F19" t="s">
         <v>29</v>
@@ -1932,7 +1992,7 @@
         <v>109</v>
       </c>
       <c r="H19">
-        <v>16.11420059204102</v>
+        <v>16.114200592041019</v>
       </c>
       <c r="I19">
         <v>2149.83544921875</v>
@@ -1941,16 +2001,16 @@
         <v>2304.625732421875</v>
       </c>
       <c r="K19">
-        <v>9.649900436401367</v>
+        <v>9.6499004364013672</v>
       </c>
       <c r="L19">
         <v>70.54620361328125</v>
       </c>
       <c r="M19">
-        <v>9.649900436401367</v>
+        <v>9.6499004364013672</v>
       </c>
       <c r="N19">
-        <v>329.3501892089844</v>
+        <v>329.35018920898438</v>
       </c>
       <c r="O19">
         <v>10.53756046295166</v>
@@ -1959,10 +2019,10 @@
         <v>1.1391761302948</v>
       </c>
       <c r="Q19">
-        <v>0.004499999806284904</v>
+        <v>4.4999998062849036E-3</v>
       </c>
       <c r="R19">
-        <v>1.4132000207901</v>
+        <v>1.4132000207901001</v>
       </c>
       <c r="S19">
         <v>16</v>
@@ -1971,7 +2031,7 @@
         <v>101</v>
       </c>
       <c r="U19">
-        <v>0.3113999962806702</v>
+        <v>0.31139999628067022</v>
       </c>
       <c r="V19">
         <v>48</v>
@@ -1980,16 +2040,16 @@
         <v>48</v>
       </c>
       <c r="X19">
-        <v>-0.0007999999797903001</v>
+        <v>-7.9999997979030013E-4</v>
       </c>
       <c r="Y19">
-        <v>149.3455047607422</v>
+        <v>149.34550476074219</v>
       </c>
       <c r="Z19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>60555</v>
       </c>
@@ -2004,7 +2064,7 @@
         <v>-36.9101</v>
       </c>
       <c r="E20">
-        <v>142.6543</v>
+        <v>142.65430000000001</v>
       </c>
       <c r="F20" t="s">
         <v>29</v>
@@ -2025,22 +2085,22 @@
         <v>15.02639961242676</v>
       </c>
       <c r="L20">
-        <v>74.97360229492188</v>
+        <v>74.973602294921875</v>
       </c>
       <c r="M20">
         <v>15.02639961242676</v>
       </c>
       <c r="N20">
-        <v>325.9736022949219</v>
+        <v>325.97360229492188</v>
       </c>
       <c r="O20">
         <v>14.77215480804443</v>
       </c>
       <c r="P20">
-        <v>0.9627653360366821</v>
+        <v>0.96276533603668213</v>
       </c>
       <c r="Q20">
-        <v>0.006399999838322401</v>
+        <v>6.399999838322401E-3</v>
       </c>
       <c r="R20">
         <v>1.418200016021729</v>
@@ -2052,7 +2112,7 @@
         <v>101</v>
       </c>
       <c r="U20">
-        <v>1.810369968414307</v>
+        <v>1.8103699684143071</v>
       </c>
       <c r="V20">
         <v>15</v>
@@ -2061,7 +2121,7 @@
         <v>90</v>
       </c>
       <c r="X20">
-        <v>-0.02309999987483025</v>
+        <v>-2.3099999874830249E-2</v>
       </c>
       <c r="Y20">
         <v>169.5863952636719</v>
@@ -2070,7 +2130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>60555</v>
       </c>
@@ -2082,7 +2142,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D21">
-        <v>-34.3252</v>
+        <v>-34.325200000000002</v>
       </c>
       <c r="E21">
         <v>142.2921</v>
@@ -2106,25 +2166,25 @@
         <v>-10.1254997253418</v>
       </c>
       <c r="L21">
-        <v>75.12550354003906</v>
+        <v>75.125503540039062</v>
       </c>
       <c r="M21">
         <v>-10.1254997253418</v>
       </c>
       <c r="N21">
-        <v>355.1318054199219</v>
+        <v>355.13180541992188</v>
       </c>
       <c r="O21">
-        <v>7.089907646179199</v>
+        <v>7.0899076461791992</v>
       </c>
       <c r="P21">
         <v>0.5764002799987793</v>
       </c>
       <c r="Q21">
-        <v>0.01130000036209822</v>
+        <v>1.130000036209822E-2</v>
       </c>
       <c r="R21">
-        <v>0.6901000142097473</v>
+        <v>0.69010001420974731</v>
       </c>
       <c r="S21">
         <v>103</v>
@@ -2133,7 +2193,7 @@
         <v>19</v>
       </c>
       <c r="U21">
-        <v>0.9775149822235107</v>
+        <v>0.97751498222351074</v>
       </c>
       <c r="V21">
         <v>9</v>
@@ -2142,7 +2202,7 @@
         <v>8</v>
       </c>
       <c r="X21">
-        <v>0.06729999929666519</v>
+        <v>6.7299999296665192E-2</v>
       </c>
       <c r="Y21">
         <v>34</v>
@@ -2151,7 +2211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>60555</v>
       </c>
@@ -2163,10 +2223,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D22">
-        <v>-35.4675</v>
+        <v>-35.467500000000001</v>
       </c>
       <c r="E22">
-        <v>143.4628</v>
+        <v>143.46279999999999</v>
       </c>
       <c r="F22" t="s">
         <v>29</v>
@@ -2175,7 +2235,7 @@
         <v>4</v>
       </c>
       <c r="H22">
-        <v>17.23609924316406</v>
+        <v>17.236099243164059</v>
       </c>
       <c r="I22">
         <v>2174.778564453125</v>
@@ -2184,28 +2244,28 @@
         <v>2247.40283203125</v>
       </c>
       <c r="K22">
-        <v>-0.179299995303154</v>
+        <v>-0.17929999530315399</v>
       </c>
       <c r="L22">
-        <v>68.17929840087891</v>
+        <v>68.179298400878906</v>
       </c>
       <c r="M22">
-        <v>-0.179299995303154</v>
+        <v>-0.17929999530315399</v>
       </c>
       <c r="N22">
-        <v>341.1825866699219</v>
+        <v>341.18258666992188</v>
       </c>
       <c r="O22">
-        <v>6.488522529602051</v>
+        <v>6.4885225296020508</v>
       </c>
       <c r="P22">
-        <v>0.623390257358551</v>
+        <v>0.62339025735855103</v>
       </c>
       <c r="Q22">
-        <v>0.000699999975040555</v>
+        <v>6.99999975040555E-4</v>
       </c>
       <c r="R22">
-        <v>1.603700041770935</v>
+        <v>1.6037000417709351</v>
       </c>
       <c r="S22">
         <v>18</v>
@@ -2214,7 +2274,7 @@
         <v>45</v>
       </c>
       <c r="U22">
-        <v>0.01624562963843346</v>
+        <v>1.624562963843346E-2</v>
       </c>
       <c r="V22">
         <v>42</v>
@@ -2223,7 +2283,7 @@
         <v>50</v>
       </c>
       <c r="X22">
-        <v>0.0006000000284984708</v>
+        <v>6.0000002849847078E-4</v>
       </c>
       <c r="Y22">
         <v>101.1999969482422</v>
@@ -2232,7 +2292,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>60555</v>
       </c>
@@ -2244,7 +2304,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D23">
-        <v>-36.4127</v>
+        <v>-36.412700000000001</v>
       </c>
       <c r="E23">
         <v>146.0248</v>
@@ -2256,7 +2316,7 @@
         <v>3</v>
       </c>
       <c r="H23">
-        <v>14.58979988098145</v>
+        <v>14.589799880981451</v>
       </c>
       <c r="I23">
         <v>2115.67626953125</v>
@@ -2265,28 +2325,28 @@
         <v>2330.111328125</v>
       </c>
       <c r="K23">
-        <v>14.27429962158203</v>
+        <v>14.274299621582029</v>
       </c>
       <c r="L23">
-        <v>74.66449737548828</v>
+        <v>74.664497375488281</v>
       </c>
       <c r="M23">
-        <v>14.27429962158203</v>
+        <v>14.274299621582029</v>
       </c>
       <c r="N23">
-        <v>345.6978149414062</v>
+        <v>345.69781494140619</v>
       </c>
       <c r="O23">
-        <v>22.13554954528809</v>
+        <v>22.135549545288089</v>
       </c>
       <c r="P23">
-        <v>3.121818542480469</v>
+        <v>3.1218185424804692</v>
       </c>
       <c r="Q23">
-        <v>0.02480000071227551</v>
+        <v>2.4800000712275509E-2</v>
       </c>
       <c r="R23">
-        <v>2.296600103378296</v>
+        <v>2.2966001033782959</v>
       </c>
       <c r="S23">
         <v>16</v>
@@ -2295,7 +2355,7 @@
         <v>68</v>
       </c>
       <c r="U23">
-        <v>0.07277580350637436</v>
+        <v>7.2775803506374359E-2</v>
       </c>
       <c r="V23">
         <v>39</v>
@@ -2304,7 +2364,7 @@
         <v>16</v>
       </c>
       <c r="X23">
-        <v>-0.1756999939680099</v>
+        <v>-0.17569999396800989</v>
       </c>
       <c r="Y23">
         <v>238.6000061035156</v>
@@ -2313,7 +2373,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>60555</v>
       </c>
@@ -2325,7 +2385,7 @@
         <v>#NUM!</v>
       </c>
       <c r="D24">
-        <v>-35.8076</v>
+        <v>-35.807600000000001</v>
       </c>
       <c r="E24">
         <v>144.3434</v>
@@ -2337,7 +2397,7 @@
         <v>103</v>
       </c>
       <c r="H24">
-        <v>16.84460067749023</v>
+        <v>16.844600677490231</v>
       </c>
       <c r="I24">
         <v>1956.269897460938</v>
@@ -2346,28 +2406,28 @@
         <v>1948.288330078125</v>
       </c>
       <c r="K24">
-        <v>-7.8649001121521</v>
+        <v>-7.8649001121520996</v>
       </c>
       <c r="L24">
-        <v>73.86489868164062</v>
+        <v>73.864898681640625</v>
       </c>
       <c r="M24">
-        <v>-7.8649001121521</v>
+        <v>-7.8649001121520996</v>
       </c>
       <c r="N24">
-        <v>351.8648986816406</v>
+        <v>351.86489868164062</v>
       </c>
       <c r="O24">
         <v>15.99424457550049</v>
       </c>
       <c r="P24">
-        <v>1.34748113155365</v>
+        <v>1.3474811315536499</v>
       </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="R24">
-        <v>1.057299971580505</v>
+        <v>1.0572999715805049</v>
       </c>
       <c r="S24">
         <v>103</v>
@@ -2376,7 +2436,7 @@
         <v>72</v>
       </c>
       <c r="U24">
-        <v>1.513473033905029</v>
+        <v>1.5134730339050291</v>
       </c>
       <c r="V24">
         <v>107</v>
@@ -2394,7 +2454,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>60555</v>
       </c>
@@ -2406,10 +2466,10 @@
         <v>#NUM!</v>
       </c>
       <c r="D25">
-        <v>-37.0163</v>
+        <v>-37.016300000000001</v>
       </c>
       <c r="E25">
-        <v>142.3824</v>
+        <v>142.38239999999999</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
@@ -2418,7 +2478,7 @@
         <v>106</v>
       </c>
       <c r="H25">
-        <v>16.26659965515137</v>
+        <v>16.266599655151371</v>
       </c>
       <c r="I25">
         <v>1838.59765625</v>
@@ -2427,16 +2487,16 @@
         <v>1855.908081054688</v>
       </c>
       <c r="K25">
-        <v>53.08700180053711</v>
+        <v>53.087001800537109</v>
       </c>
       <c r="L25">
-        <v>65.44380187988281</v>
+        <v>65.443801879882812</v>
       </c>
       <c r="M25">
-        <v>53.08700180053711</v>
+        <v>53.087001800537109</v>
       </c>
       <c r="N25">
-        <v>311.7702026367188</v>
+        <v>311.77020263671881</v>
       </c>
       <c r="O25">
         <v>7.475306510925293</v>
@@ -2445,10 +2505,10 @@
         <v>0.2490095645189285</v>
       </c>
       <c r="Q25">
-        <v>0.05209999904036522</v>
+        <v>5.2099999040365219E-2</v>
       </c>
       <c r="R25">
-        <v>2.054800033569336</v>
+        <v>2.0548000335693359</v>
       </c>
       <c r="S25">
         <v>106</v>
@@ -2466,10 +2526,10 @@
         <v>102</v>
       </c>
       <c r="X25">
-        <v>0.06530000269412994</v>
+        <v>6.5300002694129944E-2</v>
       </c>
       <c r="Y25">
-        <v>260.2000122070312</v>
+        <v>260.20001220703119</v>
       </c>
       <c r="Z25" t="s">
         <v>28</v>

</xml_diff>